<commit_message>
wheel calc. w/o base_assembly2
def.  base_assembly2
</commit_message>
<xml_diff>
--- a/RUR/BOM.xlsx
+++ b/RUR/BOM.xlsx
@@ -1,25 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_5A46845D1FA3A56933714C75F18C032DB6F14173" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C5D1C497-0C7E-4D38-A114-D681FEFFF025}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="6990" yWindow="2205" windowWidth="20280" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -42,9 +51,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>https://dk.farnell.com/tr-fastenings/4-020krst30tc1d/screw-pozi-thread-forming-m4-x/dp/2474985</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
@@ -55,16 +61,22 @@
   </si>
   <si>
     <t>Total MOQ</t>
+  </si>
+  <si>
+    <t>Ø3,5mm x 20mm countersunk self-tapping screw</t>
+  </si>
+  <si>
+    <t>link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +87,22 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,16 +125,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -120,6 +153,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>582706</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>18562</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>35857</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>36280</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="productMainImage" descr="TR FASTENINGS 3.520FLST30TC1D">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C54DDAE7-6D7E-4704-83DA-491140F4BC11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8482853" y="780562"/>
+          <a:ext cx="663386" cy="398718"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -384,11 +483,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B4:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,16 +504,16 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="H4" t="s">
         <v>3</v>
@@ -427,37 +526,74 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>60</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="3">
         <f>G5/F5</f>
         <v>0.41509999999999997</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="3">
         <f>D5*C5</f>
         <v>24.905999999999999</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="3">
         <v>100</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="3">
         <v>41.51</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>2474985</v>
       </c>
-      <c r="J5" t="s">
-        <v>7</v>
+      <c r="J5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <f>3*4+8*6</f>
+        <v>60</v>
+      </c>
+      <c r="D6" s="1">
+        <f>G6/F6</f>
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="E6" s="1">
+        <f>D6*C6</f>
+        <v>27.900000000000002</v>
+      </c>
+      <c r="F6" s="1">
+        <v>100</v>
+      </c>
+      <c r="G6" s="1">
+        <v>46.5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>2475006</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J6" r:id="rId1" xr:uid="{5DA118E4-E553-44EB-8BF5-6FC6BEA68CC8}"/>
+    <hyperlink ref="J5" r:id="rId2" xr:uid="{B94274F9-3F5B-45B6-9083-BDBDF11699F2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>